<commit_message>
Adding figures to SM in Long Paper
</commit_message>
<xml_diff>
--- a/MATLAB/results/improving_notimproving_groups_v2.xlsx
+++ b/MATLAB/results/improving_notimproving_groups_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monikaz\eth-mike-data-analysis\MATLAB\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420B5081-02AB-4F93-8442-1D43E0019DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6077DB76-71C4-4000-9949-0E463EA194A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2040" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{7452859E-D499-4473-A387-BC228B2A952B}"/>
+    <workbookView xWindow="28680" yWindow="-1935" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{7452859E-D499-4473-A387-BC228B2A952B}"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="1" r:id="rId1"/>
@@ -13055,8 +13055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2926865E-43AE-4B8E-99FA-F7474E01C92D}">
   <dimension ref="A1:AB62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X57" sqref="X57"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>